<commit_message>
correction to the best Val R^2
</commit_message>
<xml_diff>
--- a/history.xlsx
+++ b/history.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\ML Project\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB285F4C-F110-4803-8C1B-33E5DB0198B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1999A691-788C-4265-8EB0-B8C9F955BD94}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="exp" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="75">
   <si>
     <t>Kernel Size Experiment</t>
   </si>
@@ -116,36 +116,18 @@
     <t>no_aug</t>
   </si>
   <si>
-    <t>CSIRO Biomass CNN: Optimized Strategy</t>
-  </si>
-  <si>
     <t>Component</t>
   </si>
   <si>
     <t>Optimal Selection</t>
   </si>
   <si>
-    <t>Reasoning &amp; Impact</t>
-  </si>
-  <si>
-    <t>Medium Augmentation</t>
-  </si>
-  <si>
-    <t>Architecture Depth</t>
-  </si>
-  <si>
-    <t>2–3 Conv Blocks</t>
-  </si>
-  <si>
     <t>Kernel Size</t>
   </si>
   <si>
     <t>Regularization</t>
   </si>
   <si>
-    <t>Dropout 0.6 + WD 0.0001</t>
-  </si>
-  <si>
     <t>5 times 5</t>
   </si>
   <si>
@@ -155,21 +137,6 @@
     <t>3 times 3</t>
   </si>
   <si>
-    <t>Highest Avg Val R^2 (0.112); far superior to "No Augmentation" which yielded negative R^2.</t>
-  </si>
-  <si>
-    <t>Provided the most stable validation performance; 4+ blocks caused severe overfitting and loss of R^2.</t>
-  </si>
-  <si>
-    <t>Crucial for generalization; high dropout was the top-performing configuration for validation R^2.</t>
-  </si>
-  <si>
-    <t>5 times 5 Kernels</t>
-  </si>
-  <si>
-    <t>Best balance of stability (Avg Val Loss 0.132); 3 times 3 has potential but higher variance.</t>
-  </si>
-  <si>
     <t>Base Model Performance Summary</t>
   </si>
   <si>
@@ -194,13 +161,133 @@
     <t>Final Val R^2</t>
   </si>
   <si>
-    <t>Optimized Model Value</t>
-  </si>
-  <si>
     <t>Avg Train R^2</t>
   </si>
   <si>
     <t>Avg Val R^2</t>
+  </si>
+  <si>
+    <t>Final Summary Metrics</t>
+  </si>
+  <si>
+    <t>Significance</t>
+  </si>
+  <si>
+    <t>Robust training convergence.</t>
+  </si>
+  <si>
+    <t>Efficient error minimization on validation sets.</t>
+  </si>
+  <si>
+    <t>Stable baseline training performance.</t>
+  </si>
+  <si>
+    <t>Positive average generalization across all folds.</t>
+  </si>
+  <si>
+    <t>Optimized Architecture Strategy</t>
+  </si>
+  <si>
+    <t>Reasoning from Experiments</t>
+  </si>
+  <si>
+    <t>3x3</t>
+  </si>
+  <si>
+    <t>Depth</t>
+  </si>
+  <si>
+    <t>3 Conv Blocks</t>
+  </si>
+  <si>
+    <t>Dropout 0.6</t>
+  </si>
+  <si>
+    <t>Optimization</t>
+  </si>
+  <si>
+    <t>Adam + 0.0 WD</t>
+  </si>
+  <si>
+    <t>Light/Medium</t>
+  </si>
+  <si>
+    <t>Training &amp; Performance Benchmark</t>
+  </si>
+  <si>
+    <t>Metric,Optimized Baseline Value</t>
+  </si>
+  <si>
+    <t>Number of Parameters,~1.5M (approx. for 256 filters)</t>
+  </si>
+  <si>
+    <t>Avg Training Loss,0.15376</t>
+  </si>
+  <si>
+    <t>Avg Validation Loss,0.12544</t>
+  </si>
+  <si>
+    <t>Final Train R2,0.15202</t>
+  </si>
+  <si>
+    <t>Final Val R2,0.03891</t>
+  </si>
+  <si>
+    <t>Max R2 Achieved,0.32011</t>
+  </si>
+  <si>
+    <r>
+      <t>Peak Potential:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> The highest variance explained in a single run.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Best Balance:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Maintained the lowest validation loss (0.120) while capturing complex features.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Critical:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> High dropout was essential to stop the model from overfitting on small biomass samples.</t>
+    </r>
+  </si>
+  <si>
+    <t>Top Performer: Achieved the highest individual R^2 potential (0.238–0.320).</t>
+  </si>
+  <si>
+    <t>Winner: Weight Decay of 0.0 combined with high dropout yielded the best validation R^2.</t>
+  </si>
+  <si>
+    <t>Stability: Required to maintain positive R^2 values and reduce validation variance.</t>
   </si>
 </sst>
 </file>
@@ -538,8 +625,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Q14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B11" sqref="A1:XFD1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H18" sqref="H18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -641,7 +728,7 @@
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="B3" s="2">
         <v>0.15539700000000001</v>
@@ -688,7 +775,7 @@
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="B4" s="2">
         <v>0.15524199999999999</v>
@@ -735,7 +822,7 @@
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="B5" s="2">
         <v>0.147953</v>
@@ -1048,138 +1135,210 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3D7C7663-0FEB-406E-A171-49AAA11C7D81}">
-  <dimension ref="A1:D13"/>
+  <dimension ref="A1:C24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="44.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="24.77734375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="97.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="44.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.77734375" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="97.44140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="16384" width="8.88671875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
-        <v>29</v>
+        <v>46</v>
       </c>
       <c r="B1" s="4"/>
       <c r="C1" s="4"/>
-      <c r="D1" s="4"/>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="2">
+        <v>0.15376000000000001</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="2">
+        <v>0.12544</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="B5" s="2">
+        <v>0.15201999999999999</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="B6" s="2">
+        <v>3.891E-2</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="B7" s="2">
+        <v>0.32011000000000001</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A9" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="B9" s="4"/>
+      <c r="C9" s="4"/>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A10" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="B10" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="C10" s="3" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A11" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="B11" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A12" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A13" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="D2" s="2"/>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A3" s="2" t="s">
+      <c r="B13" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A14" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A15" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="B3" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="D3" s="2"/>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A4" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="D4" s="2"/>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A5" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="D5" s="2"/>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A6" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="D6" s="2"/>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A8" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="B8" s="3" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A9" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B9" s="2">
-        <v>0.170016</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A10" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B10" s="2">
-        <v>0.12705</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A11" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="B11" s="2">
-        <v>4.4748000000000003E-2</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A12" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="B12" s="2">
-        <v>3.8008E-2</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A13" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="B13" s="2">
-        <v>0.165773</v>
+      <c r="B15" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A17" s="3" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A18" s="2" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A19" s="2" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A20" s="2" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A21" s="2" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A22" s="2" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A23" s="2" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A24" s="2" t="s">
+        <v>68</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="A1:D1"/>
+  <mergeCells count="2">
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="A9:C9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1202,7 +1361,7 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="B1" s="4"/>
       <c r="C1" s="4"/>
@@ -1210,18 +1369,18 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>48</v>
+        <v>37</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>49</v>
+        <v>38</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>50</v>
+        <v>39</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>52</v>
+        <v>41</v>
       </c>
       <c r="B3">
         <v>0.2515</v>
@@ -1232,7 +1391,7 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>51</v>
+        <v>40</v>
       </c>
       <c r="B4">
         <v>0.1007</v>
@@ -1243,7 +1402,7 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>53</v>
+        <v>42</v>
       </c>
       <c r="B5">
         <v>0.34749999999999998</v>
@@ -1254,7 +1413,7 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>54</v>
+        <v>43</v>
       </c>
       <c r="B6">
         <v>0.17799999999999999</v>

</xml_diff>